<commit_message>
Fixing the students api
</commit_message>
<xml_diff>
--- a/lauCourseOffering_Backend/backend/Students _Courses.xlsx
+++ b/lauCourseOffering_Backend/backend/Students _Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1cf13879d774ffb/Desktop/Capstone/lauCourseOffering_Backend/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5A507B07-8F92-4F0F-9C75-F470DD8C9A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9EF63E1-71C9-4F07-A42A-D95CEE024B59}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{5A507B07-8F92-4F0F-9C75-F470DD8C9A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE17C47-B216-436A-8C09-024105555555}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page2_1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3363" uniqueCount="1023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3364" uniqueCount="1023">
   <si>
     <t>BIF205</t>
   </si>
@@ -3171,7 +3171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3192,10 +3192,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3534,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE821"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10703,7 +10700,9 @@
       <c r="A169" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="B169" s="8"/>
+      <c r="B169" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="C169" s="4" t="s">
         <v>80</v>
       </c>
@@ -41465,9 +41464,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:CE821" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="1">
-    <mergeCell ref="B168:B169"/>
-  </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>